<commit_message>
Minor changes in layout to main page.
</commit_message>
<xml_diff>
--- a/Group 2 - Burndown Chart.xlsx
+++ b/Group 2 - Burndown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1711971\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1715359\source\repos\Study-Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>8. Create Main page functionality</t>
+  </si>
+  <si>
+    <t>9. Create Review page</t>
+  </si>
+  <si>
+    <t>10. Create an Admin Panel</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -409,7 +415,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -418,23 +424,23 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -460,14 +466,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +585,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Study Plan App - Burndown Chart'!$B$10</c:f>
+              <c:f>'Study Plan App - Burndown Chart'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -634,36 +641,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Study Plan App - Burndown Chart'!$C$10:$K$10</c:f>
+              <c:f>'Study Plan App - Burndown Chart'!$C$12:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -680,7 +687,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Study Plan App - Burndown Chart'!$B$11</c:f>
+              <c:f>'Study Plan App - Burndown Chart'!$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -736,33 +743,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Study Plan App - Burndown Chart'!$C$11:$K$11</c:f>
+              <c:f>'Study Plan App - Burndown Chart'!$C$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.25</c:v>
+                  <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.5</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.75</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.75</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1648,13 +1655,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1940,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L13"/>
+  <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1962,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -2018,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="7">
-        <f t="shared" ref="L2:L9" si="0">SUM(D2:K2)</f>
+        <f t="shared" ref="L2:L8" si="0">SUM(D2:K2)</f>
         <v>4</v>
       </c>
     </row>
@@ -2041,10 +2048,18 @@
       <c r="G3" s="12">
         <v>1</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="13"/>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
       <c r="L3" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2055,7 +2070,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="11">
         <v>1</v>
@@ -2069,13 +2084,17 @@
       <c r="G4" s="12">
         <v>0</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="H4" s="12">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12">
+        <v>2</v>
+      </c>
       <c r="J4" s="12"/>
       <c r="K4" s="13"/>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -2097,13 +2116,15 @@
       <c r="G5" s="12">
         <v>0</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="12">
+        <v>1</v>
+      </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
       <c r="L5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -2125,13 +2146,17 @@
       <c r="G6" s="12">
         <v>0</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>3</v>
+      </c>
       <c r="J6" s="12"/>
       <c r="K6" s="13"/>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -2153,13 +2178,17 @@
       <c r="G7" s="12">
         <v>0</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="H7" s="12">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12">
+        <v>2</v>
+      </c>
       <c r="J7" s="12"/>
       <c r="K7" s="13"/>
       <c r="L7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -2190,12 +2219,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D9" s="11">
         <v>0</v>
@@ -2209,110 +2238,184 @@
       <c r="G9" s="12">
         <v>3</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
       <c r="K9" s="13"/>
-      <c r="L9" s="19">
-        <f t="shared" si="0"/>
+      <c r="L9" s="24">
+        <f>SUM(D9:K9)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="20">
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="19">
+        <f>SUM(D10:K10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="19">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="19">
+        <f>SUM(D11:K11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="25">
         <f>SUM(C2:C9)</f>
-        <v>30</v>
-      </c>
-      <c r="D10" s="14">
-        <f t="shared" ref="D10:K10" si="1">C10-SUM(D2:D9)</f>
-        <v>26</v>
-      </c>
-      <c r="E10" s="14">
+        <v>38</v>
+      </c>
+      <c r="D12" s="14">
+        <f t="shared" ref="D12:K12" si="1">C12-SUM(D2:D9)</f>
+        <v>34</v>
+      </c>
+      <c r="E12" s="14">
         <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="F10" s="14">
+        <v>31</v>
+      </c>
+      <c r="F12" s="14">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="G10" s="14">
+        <v>29</v>
+      </c>
+      <c r="G12" s="14">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="H10" s="14">
+        <v>25</v>
+      </c>
+      <c r="H12" s="14">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="I10" s="14">
+        <v>22</v>
+      </c>
+      <c r="I12" s="14">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="J10" s="14">
+        <v>15</v>
+      </c>
+      <c r="J12" s="14">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="K10" s="15">
+        <v>15</v>
+      </c>
+      <c r="K12" s="15">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C13" s="20">
         <f>SUM(C2:C9)</f>
-        <v>30</v>
-      </c>
-      <c r="D11" s="16">
-        <f t="shared" ref="D11:K11" si="2">C11-($C$10/8)</f>
-        <v>26.25</v>
-      </c>
-      <c r="E11" s="16">
+        <v>38</v>
+      </c>
+      <c r="D13" s="16">
+        <f t="shared" ref="D13:K13" si="2">C13-($C$12/8)</f>
+        <v>33.25</v>
+      </c>
+      <c r="E13" s="16">
         <f t="shared" si="2"/>
-        <v>22.5</v>
-      </c>
-      <c r="F11" s="16">
+        <v>28.5</v>
+      </c>
+      <c r="F13" s="16">
         <f t="shared" si="2"/>
-        <v>18.75</v>
-      </c>
-      <c r="G11" s="16">
+        <v>23.75</v>
+      </c>
+      <c r="G13" s="16">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="H11" s="16">
+        <v>19</v>
+      </c>
+      <c r="H13" s="16">
         <f t="shared" si="2"/>
-        <v>11.25</v>
-      </c>
-      <c r="I11" s="16">
+        <v>14.25</v>
+      </c>
+      <c r="I13" s="16">
         <f t="shared" si="2"/>
-        <v>7.5</v>
-      </c>
-      <c r="J11" s="16">
+        <v>9.5</v>
+      </c>
+      <c r="J13" s="16">
         <f t="shared" si="2"/>
-        <v>3.75</v>
-      </c>
-      <c r="K11" s="17">
+        <v>4.75</v>
+      </c>
+      <c r="K13" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+    <row r="14" spans="2:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
     </row>
-    <row r="13" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor changes to code layout and naming of various entities.
</commit_message>
<xml_diff>
--- a/Group 2 - Burndown Chart.xlsx
+++ b/Group 2 - Burndown Chart.xlsx
@@ -667,10 +667,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1950,7 +1950,7 @@
   <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,12 +2245,12 @@
         <v>0</v>
       </c>
       <c r="J9" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="24">
         <f>SUM(D9:K9)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2355,11 +2355,11 @@
       </c>
       <c r="J12" s="14">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K12" s="15">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>